<commit_message>
add images in last scrobbles page
</commit_message>
<xml_diff>
--- a/documentation/ModeleDonnees.xlsx
+++ b/documentation/ModeleDonnees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\yann\docker\myLastFm\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A4022A-2B66-4042-965F-6EFA9FF98E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7077E4-BA91-4D8B-8572-28F911D98870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15435" xr2:uid="{2ED3269A-5E17-452E-BC8D-B82D3CD96943}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,27 +669,29 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="I8" s="3" t="s">
         <v>20</v>
       </c>

</xml_diff>